<commit_message>
Added new features and UI
</commit_message>
<xml_diff>
--- a/data_renamed.xlsx
+++ b/data_renamed.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F580254F-8A2F-43E6-9521-943985976225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9917268F-E28F-4632-A9D8-40BE7230CA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,21 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>age</t>
   </si>
   <si>
     <t>sex</t>
-  </si>
-  <si>
-    <t>105, 04</t>
-  </si>
-  <si>
-    <t>105, 63</t>
-  </si>
-  <si>
-    <t>118, 57</t>
   </si>
   <si>
     <t>x1a</t>
@@ -474,7 +465,7 @@
   <dimension ref="A1:V35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,64 +488,64 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="I1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="K1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="5" t="s">
+      <c r="M1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="5" t="s">
+      <c r="O1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="5" t="s">
+      <c r="S1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" s="5" t="s">
+      <c r="V1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -872,8 +863,8 @@
       <c r="N6" s="5">
         <v>42.35</v>
       </c>
-      <c r="O6" s="5" t="s">
-        <v>2</v>
+      <c r="O6" s="5">
+        <v>105.04</v>
       </c>
       <c r="P6" s="5">
         <v>113.96</v>
@@ -1960,8 +1951,8 @@
       <c r="N22" s="5">
         <v>62.84</v>
       </c>
-      <c r="O22" s="5" t="s">
-        <v>3</v>
+      <c r="O22" s="5">
+        <v>105.63</v>
       </c>
       <c r="P22" s="5">
         <v>135.44999999999999</v>
@@ -2028,8 +2019,8 @@
       <c r="N23" s="5">
         <v>49.24</v>
       </c>
-      <c r="O23" s="5" t="s">
-        <v>4</v>
+      <c r="O23" s="5">
+        <v>118.57</v>
       </c>
       <c r="P23" s="5">
         <v>143.05000000000001</v>

</xml_diff>